<commit_message>
pre final update added
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/Data.xlsx
+++ b/target/test-classes/testdata/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kartikeysharma\Automation_QA\ExitTestFinal\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631E611E-8BC3-460B-960C-A239B63E695D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65651D09-3C3E-4B03-BD4D-5F44631E5B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>